<commit_message>
detail day in aug
</commit_message>
<xml_diff>
--- a/库存表.xlsx
+++ b/库存表.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\桌面\why so serious\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\桌面\why-so-serious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5668C5DB-602C-4563-A668-0B63E6D5471E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBDEEA5-7D06-4311-83F2-F4AC0F1236D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>货品编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,6 +100,38 @@
   </si>
   <si>
     <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线性代数严选题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武钟祥高数基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王道数据结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王道计算机组成原理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王道操作系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王道计算机网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李永乐线性代数辅导讲义</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -276,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -289,6 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,7 +619,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -615,57 +661,89 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="11">
+        <v>660</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5">
+        <v>408</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5">
+        <v>408</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5">
+        <v>408</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>408</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">

</xml_diff>